<commit_message>
Conventie rapport C# update
</commit_message>
<xml_diff>
--- a/documenten/logboeken/Logboek Jurriaan.xlsx
+++ b/documenten/logboeken/Logboek Jurriaan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Taak</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>30 min</t>
+  </si>
+  <si>
+    <t>conventies C#</t>
   </si>
 </sst>
 </file>
@@ -375,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,6 +445,17 @@
         <v>42843</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>42843</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>